<commit_message>
Deploying to gh-pages from  @ f638277711fbf02c4521faa8a57be85691786bf5 🚀
</commit_message>
<xml_diff>
--- a/2021-01-01.xlsx
+++ b/2021-01-01.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0D466C-6680-441E-9134-074F3A28F72A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20368"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projekte\Abt3_IQM-COVID19\Fachlich\Auswertungen\2021-01-01\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F597AE7B-FA28-495C-922B-94A3FF95988B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="110" windowWidth="28520" windowHeight="12600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="9" r:id="rId1"/>
-    <sheet name="30.12.20" sheetId="6" r:id="rId2"/>
+    <sheet name="31.12.20" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Bundesländer001" localSheetId="1">'30.12.20'!$A$1:$G$17</definedName>
+    <definedName name="Bundesländer001" localSheetId="1">'31.12.20'!$A$1:$G$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -27,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Bayern</t>
   </si>
@@ -101,9 +106,6 @@
     <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst die mit jeweiligem Datenstand gemeldeten Impfungen an das RKI. </t>
   </si>
   <si>
-    <t xml:space="preserve">Achtung: Die Differenz zum Vortag kann Nachmeldungen aus vorangegangenen Tagen enthalten und spiegelt nicht immer die innerhalb des Vortags tatsächlich durchgeführte Zahl der Impfungen wider. </t>
-  </si>
-  <si>
     <t>Datenstand: 28.12.2020, 08:00 Uhr</t>
   </si>
   <si>
@@ -125,7 +127,13 @@
     <t>* In einigen Bundesländern werden nicht alle der in der Tabelle aufgeführten Indikationen einzeln ausgewiesen.</t>
   </si>
   <si>
-    <t>08:30 Uhr</t>
+    <t>12:30 Uhr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achtung: Die Differenz zum Vortag kann Nachmeldungen oder Korrekturen aus vorangegangenen Tagen enthalten und spiegelt nicht immer die innerhalb des Vortags tatsächlich durchgeführte Zahl der Impfungen wider. </t>
+  </si>
+  <si>
+    <t>(für den 31.12. wurden keine Daten aus der KV-Nordrhein übermittelt)</t>
   </si>
 </sst>
 </file>
@@ -705,75 +713,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5241AA5B-8CBB-47B1-9317-352256D0A517}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="18">
         <f ca="1">TODAY()</f>
-        <v>44196</v>
+        <v>44197</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -786,20 +794,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8185A2DF-1594-45F9-85B9-EB1F8407882D}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -810,102 +818,102 @@
         <v>17</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="13">
-        <v>12649</v>
+        <v>17086</v>
       </c>
       <c r="C2" s="8">
-        <v>4407</v>
+        <v>4295</v>
       </c>
       <c r="D2" s="7">
-        <v>5347</v>
+        <v>7578</v>
       </c>
       <c r="E2" s="8">
-        <v>4196</v>
+        <v>5423</v>
       </c>
       <c r="F2" s="8">
-        <v>763</v>
+        <v>1037</v>
       </c>
       <c r="G2" s="21">
-        <v>1831</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2693</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="15">
-        <v>28206</v>
+        <v>37955</v>
       </c>
       <c r="C3" s="16">
-        <v>15104</v>
+        <v>9749</v>
       </c>
       <c r="D3" s="17">
-        <v>5831</v>
+        <v>7840</v>
       </c>
       <c r="E3" s="16">
-        <v>13981</v>
+        <v>18450</v>
       </c>
       <c r="F3" s="16">
-        <v>424</v>
+        <v>718</v>
       </c>
       <c r="G3" s="22">
-        <v>10347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>14265</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="13">
-        <v>9084</v>
+        <v>11114</v>
       </c>
       <c r="C4" s="8">
-        <v>2788</v>
+        <v>2030</v>
       </c>
       <c r="D4" s="7">
-        <v>6554</v>
+        <v>7029</v>
       </c>
       <c r="E4" s="8">
-        <v>2733</v>
+        <v>2952</v>
       </c>
       <c r="F4" s="8">
         <v>105</v>
       </c>
       <c r="G4" s="21">
-        <v>6350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="15">
-        <v>3036</v>
+        <v>3219</v>
       </c>
       <c r="C5" s="16">
-        <v>1483</v>
+        <v>183</v>
       </c>
       <c r="D5" s="17">
         <v>204</v>
       </c>
       <c r="E5" s="16">
-        <v>2812</v>
+        <v>2995</v>
       </c>
       <c r="F5" s="16">
         <v>20</v>
@@ -914,15 +922,15 @@
         <v>224</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="13">
-        <v>1691</v>
+        <v>1741</v>
       </c>
       <c r="C6" s="8">
-        <v>601</v>
+        <v>50</v>
       </c>
       <c r="D6" s="7">
         <v>821</v>
@@ -931,231 +939,234 @@
         <v>408</v>
       </c>
       <c r="F6" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G6" s="21">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="15">
-        <v>2040</v>
+        <v>2759</v>
       </c>
       <c r="C7" s="16">
-        <v>541</v>
+        <v>719</v>
       </c>
       <c r="D7" s="17">
-        <v>832</v>
+        <v>1129</v>
       </c>
       <c r="E7" s="16">
-        <v>1042</v>
+        <v>1420</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="22">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="13">
-        <v>15674</v>
+        <v>21373</v>
       </c>
       <c r="C8" s="8">
-        <v>6226</v>
+        <v>5699</v>
       </c>
       <c r="D8" s="7">
-        <v>4677</v>
+        <v>6073</v>
       </c>
       <c r="E8" s="8">
-        <v>8681</v>
+        <v>12345</v>
       </c>
       <c r="F8" s="8">
-        <v>712</v>
+        <v>821</v>
       </c>
       <c r="G8" s="21">
-        <v>6512</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8513</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="15">
-        <v>11101</v>
+        <v>11494</v>
       </c>
       <c r="C9" s="16">
-        <v>3640</v>
+        <v>393</v>
       </c>
       <c r="D9" s="17">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="E9" s="16">
-        <v>6349</v>
+        <v>6583</v>
       </c>
       <c r="F9" s="16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G9" s="22">
-        <v>4651</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4804</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="13">
-        <v>2705</v>
+        <v>3566</v>
       </c>
       <c r="C10" s="8">
-        <v>1178</v>
+        <v>861</v>
       </c>
       <c r="D10" s="7">
-        <v>296</v>
+        <v>567</v>
       </c>
       <c r="E10" s="8">
-        <v>1512</v>
+        <v>1981</v>
       </c>
       <c r="F10" s="8">
-        <v>315</v>
+        <v>654</v>
       </c>
       <c r="G10" s="21">
-        <v>1423</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="15">
-        <v>19930</v>
+        <v>24924</v>
       </c>
       <c r="C11" s="16">
-        <v>7359</v>
+        <v>3033</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="16">
-        <v>6610</v>
+        <v>8963</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="22">
-        <v>13693</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16334</v>
+      </c>
+      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="13">
-        <v>4247</v>
+        <v>5112</v>
       </c>
       <c r="C12" s="8">
-        <v>1673</v>
+        <v>865</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="8">
-        <v>1941</v>
+        <v>2329</v>
       </c>
       <c r="F12" s="8"/>
       <c r="G12" s="21">
-        <v>2306</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="15">
-        <v>2119</v>
+        <v>2716</v>
       </c>
       <c r="C13" s="16">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="D13" s="17">
-        <v>1641</v>
+        <v>2065</v>
       </c>
       <c r="E13" s="16">
-        <v>161</v>
+        <v>248</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="22">
-        <v>899</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="13">
-        <v>2653</v>
+        <v>3290</v>
       </c>
       <c r="C14" s="8">
-        <v>1166</v>
+        <v>637</v>
       </c>
       <c r="D14" s="7">
-        <v>150</v>
+        <v>226</v>
       </c>
       <c r="E14" s="8">
-        <v>2460</v>
+        <v>2754</v>
       </c>
       <c r="F14" s="8">
         <v>1</v>
       </c>
       <c r="G14" s="21">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="15">
-        <v>10100</v>
+        <v>11146</v>
       </c>
       <c r="C15" s="16">
-        <v>2813</v>
+        <v>1046</v>
       </c>
       <c r="D15" s="17">
-        <v>3107</v>
+        <v>3506</v>
       </c>
       <c r="E15" s="16">
-        <v>5068</v>
+        <v>5582</v>
       </c>
       <c r="F15" s="16">
-        <v>300</v>
+        <v>458</v>
       </c>
       <c r="G15" s="22">
-        <v>4815</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="13">
-        <v>5581</v>
+        <v>7270</v>
       </c>
       <c r="C16" s="8">
-        <v>1747</v>
+        <v>1689</v>
       </c>
       <c r="D16" s="7">
-        <v>1385</v>
+        <v>1766</v>
       </c>
       <c r="E16" s="8">
-        <v>3361</v>
+        <v>4523</v>
       </c>
       <c r="F16" s="8">
-        <v>1175</v>
+        <v>1527</v>
       </c>
       <c r="G16" s="21">
-        <v>2241</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2817</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
@@ -1163,7 +1174,7 @@
         <v>810</v>
       </c>
       <c r="C17" s="22">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D17" s="16">
         <v>232</v>
@@ -1171,48 +1182,50 @@
       <c r="E17" s="16">
         <v>297</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="16">
+        <v>0</v>
+      </c>
       <c r="G17" s="22">
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="14">
         <f>SUM(B2:B17)</f>
-        <v>131626</v>
+        <v>165575</v>
       </c>
       <c r="C18" s="14">
         <f>SUM(C2:C17)</f>
-        <v>51465</v>
+        <v>31846</v>
       </c>
       <c r="D18" s="9">
         <f t="shared" ref="D18" si="0">SUM(D2:D17)</f>
-        <v>31250</v>
+        <v>39214</v>
       </c>
       <c r="E18" s="10">
         <f>SUM(E2:E17)</f>
-        <v>61612</v>
+        <v>77253</v>
       </c>
       <c r="F18" s="10">
         <f>SUM(F2:F17)</f>
-        <v>3827</v>
+        <v>5355</v>
       </c>
       <c r="G18" s="23">
         <f>SUM(G2:G17)</f>
-        <v>57406</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>71590</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="20" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>